<commit_message>
Module: NoteButtons: added warning message before overriding cell contents, and when using the cash-back and total buttons without entering an adequate payment method
</commit_message>
<xml_diff>
--- a/Juan Alduey (Time Log and Petty Cash).xlsx
+++ b/Juan Alduey (Time Log and Petty Cash).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceciliametheny/repos/ceciliametheny/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{FBAB5D3C-4AD0-C742-8B56-9B7721AD0205}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AB65E6E8-402D-1A41-8DEB-03943C596AF7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15840" xr2:uid="{33F21683-6D57-0047-AE38-A532DA1E1845}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Refactoring code, submitting time log, determining git workflow</t>
   </si>
@@ -105,15 +105,25 @@
   <si>
     <t>Refactoring code, updating cecilia's spreadsheet, 3 month average printout of numbers</t>
   </si>
+  <si>
+    <t>fixed "clear filters" button (added error handling). Went over bills (jan to march) with cecilia to note how they were paid.</t>
+  </si>
+  <si>
+    <t>fixing note functions</t>
+  </si>
+  <si>
+    <t>Fixing note functions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="167" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -186,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -211,6 +221,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,17 +730,6 @@
             <v>2252</v>
           </cell>
         </row>
-        <row r="43">
-          <cell r="A43">
-            <v>41706</v>
-          </cell>
-          <cell r="B43" t="str">
-            <v>Lucille Metheny</v>
-          </cell>
-          <cell r="C43">
-            <v>2252</v>
-          </cell>
-        </row>
         <row r="44">
           <cell r="A44">
             <v>41707</v>
@@ -871,13 +875,13 @@
         </row>
         <row r="57">
           <cell r="A57">
-            <v>41730</v>
+            <v>41739</v>
           </cell>
           <cell r="B57" t="str">
             <v>Lucille Metheny</v>
           </cell>
           <cell r="C57">
-            <v>139.5</v>
+            <v>490.75</v>
           </cell>
         </row>
         <row r="58">
@@ -900,6 +904,50 @@
           </cell>
           <cell r="C59">
             <v>1000</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60">
+            <v>41739</v>
+          </cell>
+          <cell r="B60" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C60">
+            <v>562.25</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61">
+            <v>41739</v>
+          </cell>
+          <cell r="B61" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C61">
+            <v>380.67</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62">
+            <v>41739</v>
+          </cell>
+          <cell r="B62" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C62">
+            <v>43.4</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63">
+            <v>41727</v>
+          </cell>
+          <cell r="B63" t="str">
+            <v>The New School</v>
+          </cell>
+          <cell r="C63">
+            <v>2293.67</v>
           </cell>
         </row>
       </sheetData>
@@ -3491,13 +3539,13 @@
         </row>
         <row r="236">
           <cell r="A236">
-            <v>41710</v>
+            <v>41711</v>
           </cell>
           <cell r="B236" t="str">
-            <v>Grocery Store</v>
+            <v>Cablevision</v>
           </cell>
           <cell r="C236">
-            <v>28.29</v>
+            <v>169.46</v>
           </cell>
         </row>
         <row r="237">
@@ -3505,32 +3553,32 @@
             <v>41711</v>
           </cell>
           <cell r="B237" t="str">
-            <v>Cablevision</v>
+            <v>Consultant</v>
           </cell>
           <cell r="C237">
-            <v>169.46</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="238">
           <cell r="A238">
-            <v>41711</v>
+            <v>41713</v>
           </cell>
           <cell r="B238" t="str">
-            <v>Consultant</v>
+            <v>Body Care</v>
           </cell>
           <cell r="C238">
-            <v>20</v>
+            <v>92.7</v>
           </cell>
         </row>
         <row r="239">
           <cell r="A239">
-            <v>41713</v>
+            <v>41714</v>
           </cell>
           <cell r="B239" t="str">
-            <v>Body Care</v>
+            <v>Cleaning Supplies</v>
           </cell>
           <cell r="C239">
-            <v>92.7</v>
+            <v>22.76</v>
           </cell>
         </row>
         <row r="240">
@@ -3538,10 +3586,10 @@
             <v>41714</v>
           </cell>
           <cell r="B240" t="str">
-            <v>Cleaning Supplies</v>
+            <v>Food Out</v>
           </cell>
           <cell r="C240">
-            <v>22.76</v>
+            <v>3.95</v>
           </cell>
         </row>
         <row r="241">
@@ -3549,21 +3597,21 @@
             <v>41714</v>
           </cell>
           <cell r="B241" t="str">
-            <v>Food Out</v>
+            <v>Grocery Store</v>
           </cell>
           <cell r="C241">
-            <v>3.95</v>
+            <v>110.56</v>
           </cell>
         </row>
         <row r="242">
           <cell r="A242">
-            <v>41714</v>
+            <v>41715</v>
           </cell>
           <cell r="B242" t="str">
-            <v>Grocery Store</v>
+            <v>Donations</v>
           </cell>
           <cell r="C242">
-            <v>110.56</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="243">
@@ -3574,7 +3622,7 @@
             <v>Donations</v>
           </cell>
           <cell r="C243">
-            <v>3</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="244">
@@ -3593,10 +3641,10 @@
             <v>41715</v>
           </cell>
           <cell r="B245" t="str">
-            <v>Donations</v>
+            <v>Food Out</v>
           </cell>
           <cell r="C245">
-            <v>2</v>
+            <v>10.78</v>
           </cell>
         </row>
         <row r="246">
@@ -3607,7 +3655,7 @@
             <v>Food Out</v>
           </cell>
           <cell r="C246">
-            <v>10.78</v>
+            <v>3.26</v>
           </cell>
         </row>
         <row r="247">
@@ -3615,10 +3663,10 @@
             <v>41715</v>
           </cell>
           <cell r="B247" t="str">
-            <v>Food Out</v>
+            <v>Networking</v>
           </cell>
           <cell r="C247">
-            <v>3.26</v>
+            <v>39.200000000000003</v>
           </cell>
         </row>
         <row r="248">
@@ -3626,10 +3674,10 @@
             <v>41715</v>
           </cell>
           <cell r="B248" t="str">
-            <v>Networking</v>
+            <v>Public Transit</v>
           </cell>
           <cell r="C248">
-            <v>39.200000000000003</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="249">
@@ -3637,10 +3685,10 @@
             <v>41715</v>
           </cell>
           <cell r="B249" t="str">
-            <v>Public Transit</v>
+            <v>Taxi</v>
           </cell>
           <cell r="C249">
-            <v>3</v>
+            <v>9.36</v>
           </cell>
         </row>
         <row r="250">
@@ -3648,32 +3696,32 @@
             <v>41715</v>
           </cell>
           <cell r="B250" t="str">
-            <v>Taxi</v>
+            <v>Housekeeper</v>
           </cell>
           <cell r="C250">
-            <v>9.36</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="251">
           <cell r="A251">
-            <v>41715</v>
+            <v>41716</v>
           </cell>
           <cell r="B251" t="str">
-            <v>Housekeeper</v>
+            <v>Office Supplies</v>
           </cell>
           <cell r="C251">
-            <v>100</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="252">
           <cell r="A252">
-            <v>41716</v>
+            <v>41717</v>
           </cell>
           <cell r="B252" t="str">
-            <v>Office Supplies</v>
+            <v>Consultant</v>
           </cell>
           <cell r="C252">
-            <v>10</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="253">
@@ -3681,10 +3729,10 @@
             <v>41717</v>
           </cell>
           <cell r="B253" t="str">
-            <v>Consultant</v>
+            <v>Food Out</v>
           </cell>
           <cell r="C253">
-            <v>15</v>
+            <v>2.71</v>
           </cell>
         </row>
         <row r="254">
@@ -3692,21 +3740,21 @@
             <v>41717</v>
           </cell>
           <cell r="B254" t="str">
-            <v>Food Out</v>
+            <v>Office Supplies</v>
           </cell>
           <cell r="C254">
-            <v>2.71</v>
+            <v>24.98</v>
           </cell>
         </row>
         <row r="255">
           <cell r="A255">
-            <v>41717</v>
+            <v>41719</v>
           </cell>
           <cell r="B255" t="str">
-            <v>Office Supplies</v>
+            <v>Cell Phone</v>
           </cell>
           <cell r="C255">
-            <v>24.98</v>
+            <v>132.53</v>
           </cell>
         </row>
         <row r="256">
@@ -3714,10 +3762,10 @@
             <v>41719</v>
           </cell>
           <cell r="B256" t="str">
-            <v>Cell Phone</v>
+            <v>Household Furnishings</v>
           </cell>
           <cell r="C256">
-            <v>132.53</v>
+            <v>62.99</v>
           </cell>
         </row>
         <row r="257">
@@ -3725,10 +3773,10 @@
             <v>41719</v>
           </cell>
           <cell r="B257" t="str">
-            <v>Household Furnishings</v>
+            <v>Storage</v>
           </cell>
           <cell r="C257">
-            <v>62.99</v>
+            <v>98.33</v>
           </cell>
         </row>
         <row r="258">
@@ -3736,10 +3784,10 @@
             <v>41719</v>
           </cell>
           <cell r="B258" t="str">
-            <v>Storage</v>
+            <v>Gas Electric</v>
           </cell>
           <cell r="C258">
-            <v>98.33</v>
+            <v>238.15</v>
           </cell>
         </row>
         <row r="259">
@@ -3747,21 +3795,21 @@
             <v>41719</v>
           </cell>
           <cell r="B259" t="str">
-            <v>Gas Electric</v>
+            <v>Food Out</v>
           </cell>
           <cell r="C259">
-            <v>238.15</v>
+            <v>39.29</v>
           </cell>
         </row>
         <row r="260">
           <cell r="A260">
-            <v>41719</v>
+            <v>41720</v>
           </cell>
           <cell r="B260" t="str">
-            <v>Food Out</v>
+            <v>Body Care</v>
           </cell>
           <cell r="C260">
-            <v>39.29</v>
+            <v>72.599999999999994</v>
           </cell>
         </row>
         <row r="261">
@@ -3772,7 +3820,7 @@
             <v>Body Care</v>
           </cell>
           <cell r="C261">
-            <v>72.599999999999994</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="262">
@@ -3780,10 +3828,10 @@
             <v>41720</v>
           </cell>
           <cell r="B262" t="str">
-            <v>Body Care</v>
+            <v>Networking</v>
           </cell>
           <cell r="C262">
-            <v>20</v>
+            <v>5.93</v>
           </cell>
         </row>
         <row r="263">
@@ -3791,10 +3839,10 @@
             <v>41720</v>
           </cell>
           <cell r="B263" t="str">
-            <v>Networking</v>
+            <v>Grocery Store</v>
           </cell>
           <cell r="C263">
-            <v>5.93</v>
+            <v>5.99</v>
           </cell>
         </row>
         <row r="264">
@@ -3805,7 +3853,7 @@
             <v>Grocery Store</v>
           </cell>
           <cell r="C264">
-            <v>5.99</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="265">
@@ -3813,10 +3861,10 @@
             <v>41720</v>
           </cell>
           <cell r="B265" t="str">
-            <v>Grocery Store</v>
+            <v>Laundry</v>
           </cell>
           <cell r="C265">
-            <v>100</v>
+            <v>24</v>
           </cell>
         </row>
         <row r="266">
@@ -3824,10 +3872,10 @@
             <v>41720</v>
           </cell>
           <cell r="B266" t="str">
-            <v>Laundry</v>
+            <v>Networking</v>
           </cell>
           <cell r="C266">
-            <v>24</v>
+            <v>63.7</v>
           </cell>
         </row>
         <row r="267">
@@ -3838,7 +3886,7 @@
             <v>Networking</v>
           </cell>
           <cell r="C267">
-            <v>63.7</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="268">
@@ -3846,10 +3894,10 @@
             <v>41720</v>
           </cell>
           <cell r="B268" t="str">
-            <v>Networking</v>
+            <v>Public Transit</v>
           </cell>
           <cell r="C268">
-            <v>15</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="269">
@@ -3857,10 +3905,10 @@
             <v>41720</v>
           </cell>
           <cell r="B269" t="str">
-            <v>Public Transit</v>
+            <v>Business Travel</v>
           </cell>
           <cell r="C269">
-            <v>3</v>
+            <v>9</v>
           </cell>
         </row>
         <row r="270">
@@ -3871,7 +3919,7 @@
             <v>Business Travel</v>
           </cell>
           <cell r="C270">
-            <v>9</v>
+            <v>15.35</v>
           </cell>
         </row>
         <row r="271">
@@ -3879,10 +3927,10 @@
             <v>41720</v>
           </cell>
           <cell r="B271" t="str">
-            <v>Business Travel</v>
+            <v>Body Care</v>
           </cell>
           <cell r="C271">
-            <v>15.35</v>
+            <v>60.6</v>
           </cell>
         </row>
         <row r="272">
@@ -3893,18 +3941,18 @@
             <v>Body Care</v>
           </cell>
           <cell r="C272">
-            <v>60.6</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="273">
           <cell r="A273">
-            <v>41720</v>
+            <v>41721</v>
           </cell>
           <cell r="B273" t="str">
             <v>Body Care</v>
           </cell>
           <cell r="C273">
-            <v>12</v>
+            <v>129.56</v>
           </cell>
         </row>
         <row r="274">
@@ -3915,7 +3963,7 @@
             <v>Body Care</v>
           </cell>
           <cell r="C274">
-            <v>129.56</v>
+            <v>18.98</v>
           </cell>
         </row>
         <row r="275">
@@ -3923,10 +3971,10 @@
             <v>41721</v>
           </cell>
           <cell r="B275" t="str">
-            <v>Body Care</v>
+            <v>Food Out</v>
           </cell>
           <cell r="C275">
-            <v>18.98</v>
+            <v>16.07</v>
           </cell>
         </row>
         <row r="276">
@@ -3934,10 +3982,10 @@
             <v>41721</v>
           </cell>
           <cell r="B276" t="str">
-            <v>Food Out</v>
+            <v>Grocery Store</v>
           </cell>
           <cell r="C276">
-            <v>16.07</v>
+            <v>72.959999999999994</v>
           </cell>
         </row>
         <row r="277">
@@ -3945,10 +3993,10 @@
             <v>41721</v>
           </cell>
           <cell r="B277" t="str">
-            <v>Grocery Store</v>
+            <v>Household Furnishings</v>
           </cell>
           <cell r="C277">
-            <v>72.959999999999994</v>
+            <v>28.29</v>
           </cell>
         </row>
         <row r="278">
@@ -3956,10 +4004,10 @@
             <v>41721</v>
           </cell>
           <cell r="B278" t="str">
-            <v>Household Furnishings</v>
+            <v>Over the counter (OTC)</v>
           </cell>
           <cell r="C278">
-            <v>28.29</v>
+            <v>69.36</v>
           </cell>
         </row>
         <row r="279">
@@ -3967,10 +4015,10 @@
             <v>41721</v>
           </cell>
           <cell r="B279" t="str">
-            <v>Over the counter (OTC)</v>
+            <v>Office Supplies</v>
           </cell>
           <cell r="C279">
-            <v>69.36</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="280">
@@ -3978,10 +4026,10 @@
             <v>41721</v>
           </cell>
           <cell r="B280" t="str">
-            <v>Office Supplies</v>
+            <v>Public Transit</v>
           </cell>
           <cell r="C280">
-            <v>16</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="281">
@@ -3989,10 +4037,10 @@
             <v>41721</v>
           </cell>
           <cell r="B281" t="str">
-            <v>Public Transit</v>
+            <v>Flowers</v>
           </cell>
           <cell r="C281">
-            <v>3</v>
+            <v>21.65</v>
           </cell>
         </row>
         <row r="282">
@@ -4000,10 +4048,10 @@
             <v>41721</v>
           </cell>
           <cell r="B282" t="str">
-            <v>Flowers</v>
+            <v>Body Care</v>
           </cell>
           <cell r="C282">
-            <v>21.65</v>
+            <v>18.88</v>
           </cell>
         </row>
         <row r="283">
@@ -4011,10 +4059,10 @@
             <v>41721</v>
           </cell>
           <cell r="B283" t="str">
-            <v>Body Care</v>
+            <v>Laundry</v>
           </cell>
           <cell r="C283">
-            <v>18.88</v>
+            <v>24</v>
           </cell>
         </row>
         <row r="284">
@@ -4022,15 +4070,15 @@
             <v>41721</v>
           </cell>
           <cell r="B284" t="str">
-            <v>Laundry</v>
+            <v>Household Furnishings</v>
           </cell>
           <cell r="C284">
-            <v>24</v>
+            <v>16.329999999999998</v>
           </cell>
         </row>
         <row r="285">
           <cell r="A285">
-            <v>41721</v>
+            <v>41723</v>
           </cell>
           <cell r="B285" t="str">
             <v>Networking</v>
@@ -4041,13 +4089,13 @@
         </row>
         <row r="286">
           <cell r="A286">
-            <v>41721</v>
+            <v>41723</v>
           </cell>
           <cell r="B286" t="str">
-            <v>Household Furnishings</v>
+            <v>Flowers</v>
           </cell>
           <cell r="C286">
-            <v>16.329999999999998</v>
+            <v>21.65</v>
           </cell>
         </row>
         <row r="287">
@@ -4055,43 +4103,37 @@
             <v>41723</v>
           </cell>
           <cell r="B287" t="str">
-            <v>Networking</v>
+            <v>Parsons</v>
           </cell>
           <cell r="C287">
-            <v>60.26</v>
+            <v>9.35</v>
           </cell>
         </row>
         <row r="288">
           <cell r="A288">
-            <v>41723</v>
-          </cell>
-          <cell r="B288" t="str">
-            <v>Flowers</v>
+            <v>41724</v>
           </cell>
           <cell r="C288">
-            <v>21.65</v>
+            <v>13.32</v>
           </cell>
         </row>
         <row r="289">
           <cell r="A289">
-            <v>41723</v>
+            <v>41724</v>
           </cell>
           <cell r="B289" t="str">
-            <v>Parsons</v>
+            <v>Cleaning Supplies</v>
           </cell>
           <cell r="C289">
-            <v>9.35</v>
+            <v>14.99</v>
           </cell>
         </row>
         <row r="290">
           <cell r="A290">
             <v>41724</v>
           </cell>
-          <cell r="B290" t="str">
-            <v>Flowers</v>
-          </cell>
           <cell r="C290">
-            <v>13.32</v>
+            <v>1.99</v>
           </cell>
         </row>
         <row r="291">
@@ -4099,10 +4141,10 @@
             <v>41724</v>
           </cell>
           <cell r="B291" t="str">
-            <v>Cleaning Supplies</v>
+            <v>Grocery Store</v>
           </cell>
           <cell r="C291">
-            <v>14.99</v>
+            <v>30.3</v>
           </cell>
         </row>
         <row r="292">
@@ -4110,21 +4152,21 @@
             <v>41724</v>
           </cell>
           <cell r="B292" t="str">
-            <v>Body Care</v>
+            <v>Bank Fee</v>
           </cell>
           <cell r="C292">
-            <v>1.99</v>
+            <v>70</v>
           </cell>
         </row>
         <row r="293">
           <cell r="A293">
-            <v>41724</v>
+            <v>41725</v>
           </cell>
           <cell r="B293" t="str">
-            <v>Grocery Store</v>
+            <v>Bank Fee</v>
           </cell>
           <cell r="C293">
-            <v>30.3</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="294">
@@ -4132,10 +4174,10 @@
             <v>41725</v>
           </cell>
           <cell r="B294" t="str">
-            <v>Bank Fee</v>
+            <v>Gardening</v>
           </cell>
           <cell r="C294">
-            <v>3</v>
+            <v>190.67</v>
           </cell>
         </row>
         <row r="295">
@@ -4143,21 +4185,21 @@
             <v>41725</v>
           </cell>
           <cell r="B295" t="str">
-            <v>Gardening</v>
+            <v>Grocery Store</v>
           </cell>
           <cell r="C295">
-            <v>190.67</v>
+            <v>62.49</v>
           </cell>
         </row>
         <row r="296">
           <cell r="A296">
-            <v>41725</v>
+            <v>41726</v>
           </cell>
           <cell r="B296" t="str">
-            <v>Grocery Store</v>
+            <v>CHASE Amazon v5475</v>
           </cell>
           <cell r="C296">
-            <v>62.49</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="297">
@@ -4165,10 +4207,10 @@
             <v>41726</v>
           </cell>
           <cell r="B297" t="str">
-            <v>CHASE Amazon v5475</v>
+            <v>Bank Fee</v>
           </cell>
           <cell r="C297">
-            <v>500</v>
+            <v>1.5</v>
           </cell>
         </row>
         <row r="298">
@@ -4176,10 +4218,10 @@
             <v>41726</v>
           </cell>
           <cell r="B298" t="str">
-            <v>Bank Fee</v>
+            <v>First Premier MC 3141</v>
           </cell>
           <cell r="C298">
-            <v>1.5</v>
+            <v>346.22</v>
           </cell>
         </row>
         <row r="299">
@@ -4187,21 +4229,21 @@
             <v>41726</v>
           </cell>
           <cell r="B299" t="str">
-            <v>First Premier MC 3141</v>
+            <v>Public Transit</v>
           </cell>
           <cell r="C299">
-            <v>346.22</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="300">
           <cell r="A300">
-            <v>41726</v>
+            <v>41727</v>
           </cell>
           <cell r="B300" t="str">
-            <v>Public Transit</v>
+            <v>Parsons</v>
           </cell>
           <cell r="C300">
-            <v>3</v>
+            <v>39.14</v>
           </cell>
         </row>
         <row r="301">
@@ -4209,10 +4251,10 @@
             <v>41727</v>
           </cell>
           <cell r="B301" t="str">
-            <v>Parsons</v>
+            <v>Food Out</v>
           </cell>
           <cell r="C301">
-            <v>39.14</v>
+            <v>8.84</v>
           </cell>
         </row>
         <row r="302">
@@ -4220,10 +4262,10 @@
             <v>41727</v>
           </cell>
           <cell r="B302" t="str">
-            <v>Food Out</v>
+            <v>household Furnishings</v>
           </cell>
           <cell r="C302">
-            <v>8.84</v>
+            <v>9.3000000000000007</v>
           </cell>
         </row>
         <row r="303">
@@ -4231,10 +4273,10 @@
             <v>41727</v>
           </cell>
           <cell r="B303" t="str">
-            <v>household Furnishings</v>
+            <v>Federal Taxes</v>
           </cell>
           <cell r="C303">
-            <v>9.3000000000000007</v>
+            <v>108.53</v>
           </cell>
         </row>
         <row r="304">
@@ -4242,21 +4284,21 @@
             <v>41727</v>
           </cell>
           <cell r="B304" t="str">
-            <v>Federal Taxes</v>
+            <v>Networking</v>
           </cell>
           <cell r="C304">
-            <v>108.53</v>
+            <v>14.35</v>
           </cell>
         </row>
         <row r="305">
           <cell r="A305">
-            <v>41727</v>
+            <v>41729</v>
           </cell>
           <cell r="B305" t="str">
-            <v>Networking</v>
+            <v>Rent</v>
           </cell>
           <cell r="C305">
-            <v>14.35</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="306">
@@ -4264,10 +4306,10 @@
             <v>41729</v>
           </cell>
           <cell r="B306" t="str">
-            <v>Rent</v>
+            <v>Donations</v>
           </cell>
           <cell r="C306">
-            <v>1000</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="307">
@@ -4278,7 +4320,7 @@
             <v>Donations</v>
           </cell>
           <cell r="C307">
-            <v>3</v>
+            <v>2.5</v>
           </cell>
         </row>
         <row r="308">
@@ -4286,10 +4328,10 @@
             <v>41729</v>
           </cell>
           <cell r="B308" t="str">
-            <v>Donations</v>
+            <v>Networking</v>
           </cell>
           <cell r="C308">
-            <v>2.5</v>
+            <v>31.65</v>
           </cell>
         </row>
         <row r="309">
@@ -4297,21 +4339,21 @@
             <v>41729</v>
           </cell>
           <cell r="B309" t="str">
-            <v>Networking</v>
+            <v>Go Daddy</v>
           </cell>
           <cell r="C309">
-            <v>31.65</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="310">
           <cell r="A310">
-            <v>41729</v>
+            <v>41730</v>
           </cell>
           <cell r="B310" t="str">
-            <v>Go Daddy</v>
+            <v>Credit One MC4850</v>
           </cell>
           <cell r="C310">
-            <v>15</v>
+            <v>139.5</v>
           </cell>
         </row>
         <row r="311">
@@ -4319,10 +4361,10 @@
             <v>41730</v>
           </cell>
           <cell r="B311" t="str">
-            <v>Credit One MC4850</v>
+            <v>Credit One V7030</v>
           </cell>
           <cell r="C311">
-            <v>139.5</v>
+            <v>153.13</v>
           </cell>
         </row>
         <row r="312">
@@ -4330,10 +4372,10 @@
             <v>41730</v>
           </cell>
           <cell r="B312" t="str">
-            <v>Credit One V7030</v>
+            <v>Apartment Insurance (State Farm)</v>
           </cell>
           <cell r="C312">
-            <v>153.13</v>
+            <v>25.25</v>
           </cell>
         </row>
         <row r="313">
@@ -4341,32 +4383,32 @@
             <v>41730</v>
           </cell>
           <cell r="B313" t="str">
-            <v>Apartment Insurance (State Farm)</v>
+            <v>Google Cloud Service</v>
           </cell>
           <cell r="C313">
-            <v>25.25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="314">
           <cell r="A314">
-            <v>41730</v>
+            <v>41731</v>
           </cell>
           <cell r="B314" t="str">
-            <v>Google Cloud Service</v>
+            <v>Consultant</v>
           </cell>
           <cell r="C314">
-            <v>15</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="315">
           <cell r="A315">
-            <v>41731</v>
+            <v>41732</v>
           </cell>
           <cell r="B315" t="str">
-            <v>Consultant</v>
+            <v>Grocery Store</v>
           </cell>
           <cell r="C315">
-            <v>1000</v>
+            <v>50.15</v>
           </cell>
         </row>
         <row r="316">
@@ -4374,10 +4416,10 @@
             <v>41732</v>
           </cell>
           <cell r="B316" t="str">
-            <v>Grocery Store</v>
+            <v>Flowers</v>
           </cell>
           <cell r="C316">
-            <v>50.15</v>
+            <v>12.98</v>
           </cell>
         </row>
         <row r="317">
@@ -4385,10 +4427,10 @@
             <v>41732</v>
           </cell>
           <cell r="B317" t="str">
-            <v>Flowers</v>
+            <v>Food Out</v>
           </cell>
           <cell r="C317">
-            <v>12.98</v>
+            <v>15.09</v>
           </cell>
         </row>
         <row r="318">
@@ -4396,10 +4438,10 @@
             <v>41732</v>
           </cell>
           <cell r="B318" t="str">
-            <v>Food Out</v>
+            <v>Networking</v>
           </cell>
           <cell r="C318">
-            <v>15.09</v>
+            <v>20.420000000000002</v>
           </cell>
         </row>
         <row r="319">
@@ -4407,10 +4449,10 @@
             <v>41732</v>
           </cell>
           <cell r="B319" t="str">
-            <v>Networking</v>
+            <v>Parsons</v>
           </cell>
           <cell r="C319">
-            <v>20.420000000000002</v>
+            <v>13.34</v>
           </cell>
         </row>
         <row r="320">
@@ -4418,10 +4460,10 @@
             <v>41732</v>
           </cell>
           <cell r="B320" t="str">
-            <v>Parsons</v>
+            <v>Clothes</v>
           </cell>
           <cell r="C320">
-            <v>13.34</v>
+            <v>47.6</v>
           </cell>
         </row>
         <row r="321">
@@ -4429,21 +4471,21 @@
             <v>41732</v>
           </cell>
           <cell r="B321" t="str">
-            <v>Clothes</v>
+            <v>Public Transit</v>
           </cell>
           <cell r="C321">
-            <v>47.6</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="322">
           <cell r="A322">
-            <v>41732</v>
+            <v>41733</v>
           </cell>
           <cell r="B322" t="str">
-            <v>Public Transit</v>
+            <v>Medical</v>
           </cell>
           <cell r="C322">
-            <v>3</v>
+            <v>90</v>
           </cell>
         </row>
         <row r="323">
@@ -4451,10 +4493,10 @@
             <v>41733</v>
           </cell>
           <cell r="B323" t="str">
-            <v>Medical</v>
+            <v>Grocery Store</v>
           </cell>
           <cell r="C323">
-            <v>90</v>
+            <v>39.67</v>
           </cell>
         </row>
         <row r="324">
@@ -4462,10 +4504,10 @@
             <v>41733</v>
           </cell>
           <cell r="B324" t="str">
-            <v>Grocery Store</v>
+            <v>Wine</v>
           </cell>
           <cell r="C324">
-            <v>39.67</v>
+            <v>19.59</v>
           </cell>
         </row>
         <row r="325">
@@ -4473,10 +4515,10 @@
             <v>41733</v>
           </cell>
           <cell r="B325" t="str">
-            <v>Wine</v>
+            <v>Food Out</v>
           </cell>
           <cell r="C325">
-            <v>19.59</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="326">
@@ -4484,10 +4526,10 @@
             <v>41733</v>
           </cell>
           <cell r="B326" t="str">
-            <v>Food Out</v>
+            <v>Public Transit</v>
           </cell>
           <cell r="C326">
-            <v>6</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="327">
@@ -4495,21 +4537,21 @@
             <v>41733</v>
           </cell>
           <cell r="B327" t="str">
-            <v>Public Transit</v>
+            <v>Networking</v>
           </cell>
           <cell r="C327">
-            <v>3</v>
+            <v>165.5</v>
           </cell>
         </row>
         <row r="328">
           <cell r="A328">
-            <v>41733</v>
+            <v>41734</v>
           </cell>
           <cell r="B328" t="str">
-            <v>Parsons</v>
+            <v>Gas Electric</v>
           </cell>
           <cell r="C328">
-            <v>165.5</v>
+            <v>306.62</v>
           </cell>
         </row>
         <row r="329">
@@ -4517,10 +4559,10 @@
             <v>41734</v>
           </cell>
           <cell r="B329" t="str">
-            <v>Gas Electric</v>
+            <v>Lucille Metheny</v>
           </cell>
           <cell r="C329">
-            <v>306.62</v>
+            <v>28</v>
           </cell>
         </row>
         <row r="330">
@@ -4528,10 +4570,10 @@
             <v>41734</v>
           </cell>
           <cell r="B330" t="str">
-            <v>Lucille Metheny</v>
+            <v>Food Out</v>
           </cell>
           <cell r="C330">
-            <v>28</v>
+            <v>8.33</v>
           </cell>
         </row>
         <row r="331">
@@ -4539,10 +4581,10 @@
             <v>41734</v>
           </cell>
           <cell r="B331" t="str">
-            <v>Food Out</v>
+            <v>Public Transit</v>
           </cell>
           <cell r="C331">
-            <v>8.33</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="332">
@@ -4553,18 +4595,18 @@
             <v>Public Transit</v>
           </cell>
           <cell r="C332">
-            <v>3</v>
+            <v>13.95</v>
           </cell>
         </row>
         <row r="333">
           <cell r="A333">
-            <v>41734</v>
+            <v>41735</v>
           </cell>
           <cell r="B333" t="str">
-            <v>Public Transit</v>
+            <v>Laundry</v>
           </cell>
           <cell r="C333">
-            <v>13.95</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="334">
@@ -4572,10 +4614,10 @@
             <v>41735</v>
           </cell>
           <cell r="B334" t="str">
-            <v>Laundry</v>
+            <v>Grocery Store</v>
           </cell>
           <cell r="C334">
-            <v>16</v>
+            <v>58.7</v>
           </cell>
         </row>
         <row r="335">
@@ -4583,10 +4625,10 @@
             <v>41735</v>
           </cell>
           <cell r="B335" t="str">
-            <v>Grocery Store</v>
+            <v>Cleaning Supplies</v>
           </cell>
           <cell r="C335">
-            <v>58.7</v>
+            <v>10.49</v>
           </cell>
         </row>
         <row r="336">
@@ -4594,10 +4636,10 @@
             <v>41735</v>
           </cell>
           <cell r="B336" t="str">
-            <v>Cleaning Supplies</v>
+            <v>Parsons</v>
           </cell>
           <cell r="C336">
-            <v>10.49</v>
+            <v>4.99</v>
           </cell>
         </row>
         <row r="337">
@@ -4605,10 +4647,10 @@
             <v>41735</v>
           </cell>
           <cell r="B337" t="str">
-            <v>Parsons</v>
+            <v>Body Care</v>
           </cell>
           <cell r="C337">
-            <v>4.99</v>
+            <v>18.95</v>
           </cell>
         </row>
         <row r="338">
@@ -4616,10 +4658,10 @@
             <v>41735</v>
           </cell>
           <cell r="B338" t="str">
-            <v>Body Care</v>
+            <v>Food Out</v>
           </cell>
           <cell r="C338">
-            <v>18.95</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="339">
@@ -4630,18 +4672,18 @@
             <v>Food Out</v>
           </cell>
           <cell r="C339">
-            <v>2</v>
+            <v>10.46</v>
           </cell>
         </row>
         <row r="340">
           <cell r="A340">
-            <v>41735</v>
+            <v>41736</v>
           </cell>
           <cell r="B340" t="str">
             <v>Food Out</v>
           </cell>
           <cell r="C340">
-            <v>10.46</v>
+            <v>41.67</v>
           </cell>
         </row>
         <row r="341">
@@ -4652,7 +4694,7 @@
             <v>Food Out</v>
           </cell>
           <cell r="C341">
-            <v>41.67</v>
+            <v>3.26</v>
           </cell>
         </row>
         <row r="342">
@@ -4660,10 +4702,10 @@
             <v>41736</v>
           </cell>
           <cell r="B342" t="str">
-            <v>Food Out</v>
+            <v>Public Transit</v>
           </cell>
           <cell r="C342">
-            <v>3.26</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="343">
@@ -4671,10 +4713,10 @@
             <v>41736</v>
           </cell>
           <cell r="B343" t="str">
-            <v>Public Transit</v>
+            <v>Food Out</v>
           </cell>
           <cell r="C343">
-            <v>3</v>
+            <v>20.54</v>
           </cell>
         </row>
         <row r="344">
@@ -4682,10 +4724,10 @@
             <v>41736</v>
           </cell>
           <cell r="B344" t="str">
-            <v>Food Out</v>
+            <v>Body Care</v>
           </cell>
           <cell r="C344">
-            <v>20.54</v>
+            <v>34.6</v>
           </cell>
         </row>
         <row r="345">
@@ -4696,7 +4738,7 @@
             <v>Body Care</v>
           </cell>
           <cell r="C345">
-            <v>34.6</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="346">
@@ -4704,10 +4746,10 @@
             <v>41736</v>
           </cell>
           <cell r="B346" t="str">
-            <v>Body Care</v>
+            <v>Grocery Store</v>
           </cell>
           <cell r="C346">
-            <v>10</v>
+            <v>22.88</v>
           </cell>
         </row>
         <row r="347">
@@ -4715,10 +4757,10 @@
             <v>41736</v>
           </cell>
           <cell r="B347" t="str">
-            <v>Grocery Store</v>
+            <v>Food Out</v>
           </cell>
           <cell r="C347">
-            <v>22.88</v>
+            <v>38.67</v>
           </cell>
         </row>
         <row r="348">
@@ -4729,7 +4771,7 @@
             <v>Food Out</v>
           </cell>
           <cell r="C348">
-            <v>36.67</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="349">
@@ -4740,18 +4782,246 @@
             <v>Food Out</v>
           </cell>
           <cell r="C349">
-            <v>3</v>
+            <v>3.26</v>
           </cell>
         </row>
         <row r="350">
           <cell r="A350">
-            <v>41736</v>
+            <v>41737</v>
           </cell>
           <cell r="B350" t="str">
+            <v>Life Insurance (AARP)</v>
+          </cell>
+          <cell r="C350">
+            <v>26.38</v>
+          </cell>
+        </row>
+        <row r="351">
+          <cell r="A351">
+            <v>41737</v>
+          </cell>
+          <cell r="B351" t="str">
+            <v>Taxi</v>
+          </cell>
+          <cell r="C351">
+            <v>13.56</v>
+          </cell>
+        </row>
+        <row r="352">
+          <cell r="A352">
+            <v>41737</v>
+          </cell>
+          <cell r="B352" t="str">
+            <v>Wine</v>
+          </cell>
+          <cell r="C352">
+            <v>19.59</v>
+          </cell>
+        </row>
+        <row r="353">
+          <cell r="A353">
+            <v>41737</v>
+          </cell>
+          <cell r="B353" t="str">
+            <v>Medical</v>
+          </cell>
+          <cell r="C353">
+            <v>90</v>
+          </cell>
+        </row>
+        <row r="354">
+          <cell r="A354">
+            <v>41738</v>
+          </cell>
+          <cell r="B354" t="str">
+            <v>Grocery Store</v>
+          </cell>
+          <cell r="C354">
+            <v>51.98</v>
+          </cell>
+        </row>
+        <row r="355">
+          <cell r="A355">
+            <v>41738</v>
+          </cell>
+          <cell r="B355" t="str">
+            <v>Over the counter (OTC)</v>
+          </cell>
+          <cell r="C355">
+            <v>11.98</v>
+          </cell>
+        </row>
+        <row r="356">
+          <cell r="A356">
+            <v>41738</v>
+          </cell>
+          <cell r="B356" t="str">
+            <v>Public Transit</v>
+          </cell>
+          <cell r="C356">
+            <v>20</v>
+          </cell>
+        </row>
+        <row r="357">
+          <cell r="A357">
+            <v>41738</v>
+          </cell>
+          <cell r="C357">
+            <v>53.93</v>
+          </cell>
+        </row>
+        <row r="358">
+          <cell r="A358">
+            <v>41738</v>
+          </cell>
+          <cell r="B358" t="str">
             <v>Food Out</v>
           </cell>
-          <cell r="C350">
-            <v>3.26</v>
+          <cell r="C358">
+            <v>10.69</v>
+          </cell>
+        </row>
+        <row r="359">
+          <cell r="A359">
+            <v>41739</v>
+          </cell>
+          <cell r="B359" t="str">
+            <v>Medical</v>
+          </cell>
+          <cell r="C359">
+            <v>110.57</v>
+          </cell>
+        </row>
+        <row r="360">
+          <cell r="A360">
+            <v>41739</v>
+          </cell>
+          <cell r="B360" t="str">
+            <v>Public Transit</v>
+          </cell>
+          <cell r="C360">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="361">
+          <cell r="A361">
+            <v>41739</v>
+          </cell>
+          <cell r="B361" t="str">
+            <v>Food Out</v>
+          </cell>
+          <cell r="C361">
+            <v>12.72</v>
+          </cell>
+        </row>
+        <row r="362">
+          <cell r="A362">
+            <v>41739</v>
+          </cell>
+          <cell r="B362" t="str">
+            <v>Consultant</v>
+          </cell>
+          <cell r="C362">
+            <v>562.25</v>
+          </cell>
+        </row>
+        <row r="363">
+          <cell r="A363">
+            <v>41739</v>
+          </cell>
+          <cell r="B363" t="str">
+            <v>Taxi</v>
+          </cell>
+          <cell r="C363">
+            <v>15.35</v>
+          </cell>
+        </row>
+        <row r="364">
+          <cell r="A364">
+            <v>41739</v>
+          </cell>
+          <cell r="B364" t="str">
+            <v>Gift</v>
+          </cell>
+          <cell r="C364">
+            <v>14.15</v>
+          </cell>
+        </row>
+        <row r="365">
+          <cell r="A365">
+            <v>41739</v>
+          </cell>
+          <cell r="B365" t="str">
+            <v>Cell Phone</v>
+          </cell>
+          <cell r="C365">
+            <v>133.53</v>
+          </cell>
+        </row>
+        <row r="366">
+          <cell r="A366">
+            <v>41739</v>
+          </cell>
+          <cell r="B366" t="str">
+            <v>Accessories</v>
+          </cell>
+          <cell r="C366">
+            <v>380.67</v>
+          </cell>
+        </row>
+        <row r="367">
+          <cell r="A367">
+            <v>41739</v>
+          </cell>
+          <cell r="B367" t="str">
+            <v>Accessories</v>
+          </cell>
+          <cell r="C367">
+            <v>43.4</v>
+          </cell>
+        </row>
+        <row r="368">
+          <cell r="A368">
+            <v>41739</v>
+          </cell>
+          <cell r="B368" t="str">
+            <v>Entertainment Subscription</v>
+          </cell>
+          <cell r="C368">
+            <v>1.61</v>
+          </cell>
+        </row>
+        <row r="369">
+          <cell r="A369">
+            <v>41739</v>
+          </cell>
+          <cell r="B369" t="str">
+            <v>Entertainment Subscription</v>
+          </cell>
+          <cell r="C369">
+            <v>4.99</v>
+          </cell>
+        </row>
+        <row r="370">
+          <cell r="A370">
+            <v>41739</v>
+          </cell>
+          <cell r="B370" t="str">
+            <v>Public Transit</v>
+          </cell>
+          <cell r="C370">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="371">
+          <cell r="A371">
+            <v>41740</v>
+          </cell>
+          <cell r="B371" t="str">
+            <v>Office Supplies</v>
+          </cell>
+          <cell r="C371">
+            <v>38.520000000000003</v>
           </cell>
         </row>
       </sheetData>
@@ -5050,8 +5320,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5355,17 +5625,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2C0C1C-0C1B-0F47-B63F-0FE5E619F129}">
   <sheetPr codeName="Sheet6" filterMode="1"/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" style="15" customWidth="1"/>
     <col min="2" max="2" width="16" style="15" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="15"/>
+    <col min="3" max="3" width="11.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="2"/>
     <col min="5" max="5" width="25.5" style="1" customWidth="1"/>
   </cols>
@@ -5398,7 +5668,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ref="D2:D19" si="0">(C2-B2)*24</f>
+        <f t="shared" ref="D2:D23" si="0">(C2-B2)*24</f>
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -5711,13 +5981,94 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>43206</v>
       </c>
       <c r="B20" s="3">
         <v>0.51597222222222217</v>
       </c>
+      <c r="C20" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>3.2166666666666686</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>43207</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>1.6333333333333329</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>43207</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.52013888888888882</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.68680555555555556</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000018</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>43208</v>
+      </c>
+      <c r="B23" s="3">
+        <v>9.4444444444444442E-2</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.15277777777777776</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3999999999999997</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>43215</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.56736111111111109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="16"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="17"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E18" xr:uid="{83D46876-B0DE-D146-A3B3-758CD4F9A470}">
@@ -5737,10 +6088,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93AF818-D70E-9E47-9D21-C62781B34393}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5821,7 +6172,7 @@
       </c>
       <c r="F8" s="8">
         <f>SUM(B:B)</f>
-        <v>11.45</v>
+        <v>25.45</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -5977,6 +6328,30 @@
       </c>
       <c r="B27" s="6">
         <v>-7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28" s="18">
+        <v>43206</v>
+      </c>
+      <c r="B28" s="6">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" s="7">
+        <v>43207</v>
+      </c>
+      <c r="B29" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" s="7">
+        <v>43207</v>
+      </c>
+      <c r="B30" s="6">
+        <v>-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made code more readable usint With statements; fixed Lucille Metheny buttons
</commit_message>
<xml_diff>
--- a/Juan Alduey (Time Log and Petty Cash).xlsx
+++ b/Juan Alduey (Time Log and Petty Cash).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceciliametheny/repos/ceciliametheny/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AB65E6E8-402D-1A41-8DEB-03943C596AF7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{71A4F3EA-8CDA-824E-8586-5D969F422DD7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15840" xr2:uid="{33F21683-6D57-0047-AE38-A532DA1E1845}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15840" activeTab="1" xr2:uid="{33F21683-6D57-0047-AE38-A532DA1E1845}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeLog" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Refactoring code, submitting time log, determining git workflow</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Fixing note functions</t>
+  </si>
+  <si>
+    <t>fix note functions and update links warning message</t>
   </si>
 </sst>
 </file>
@@ -5627,8 +5630,8 @@
   <sheetPr codeName="Sheet6" filterMode="1"/>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -5668,7 +5671,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ref="D2:D23" si="0">(C2-B2)*24</f>
+        <f t="shared" ref="D2:D24" si="0">(C2-B2)*24</f>
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -6053,12 +6056,30 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>43215</v>
       </c>
       <c r="B24" s="3">
-        <v>0.56736111111111109</v>
+        <v>0.61875000000000002</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.65069444444444446</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.76666666666666661</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>43216</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.52083333333333337</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -6088,10 +6109,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93AF818-D70E-9E47-9D21-C62781B34393}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6172,7 +6193,7 @@
       </c>
       <c r="F8" s="8">
         <f>SUM(B:B)</f>
-        <v>25.45</v>
+        <v>18.45</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -6352,6 +6373,14 @@
       </c>
       <c r="B30" s="6">
         <v>-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" s="7">
+        <v>43216</v>
+      </c>
+      <c r="B31" s="6">
+        <v>-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Collapsed LM transactioins down to a single step
</commit_message>
<xml_diff>
--- a/Juan Alduey (Time Log and Petty Cash).xlsx
+++ b/Juan Alduey (Time Log and Petty Cash).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceciliametheny/repos/ceciliametheny/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{71A4F3EA-8CDA-824E-8586-5D969F422DD7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{76FA4691-D726-BC46-AF3A-1CC6FA704EC5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15840" activeTab="1" xr2:uid="{33F21683-6D57-0047-AE38-A532DA1E1845}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15840" xr2:uid="{33F21683-6D57-0047-AE38-A532DA1E1845}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeLog" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Refactoring code, submitting time log, determining git workflow</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>fix note functions and update links warning message</t>
+  </si>
+  <si>
+    <t>Fixed visa, date, and category buttons, plus data validation issue with LM transactions.</t>
   </si>
 </sst>
 </file>
@@ -944,10 +947,10 @@
         </row>
         <row r="63">
           <cell r="A63">
-            <v>41727</v>
+            <v>41752</v>
           </cell>
           <cell r="B63" t="str">
-            <v>The New School</v>
+            <v>CeMe</v>
           </cell>
           <cell r="C63">
             <v>2293.67</v>
@@ -5025,6 +5028,17 @@
           </cell>
           <cell r="C371">
             <v>38.520000000000003</v>
+          </cell>
+        </row>
+        <row r="372">
+          <cell r="A372">
+            <v>41753</v>
+          </cell>
+          <cell r="B372" t="str">
+            <v>Food Out</v>
+          </cell>
+          <cell r="C372">
+            <v>35</v>
           </cell>
         </row>
       </sheetData>
@@ -5630,8 +5644,8 @@
   <sheetPr codeName="Sheet6" filterMode="1"/>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -5671,7 +5685,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ref="D2:D24" si="0">(C2-B2)*24</f>
+        <f t="shared" ref="D2:D25" si="0">(C2-B2)*24</f>
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -6074,12 +6088,30 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>43216</v>
       </c>
       <c r="B25" s="3">
         <v>0.52083333333333337</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.67083333333333339</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>3.6000000000000005</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>43220</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.44236111111111115</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -6111,7 +6143,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added/fixed error handling for LM buttons.
</commit_message>
<xml_diff>
--- a/Juan Alduey (Time Log and Petty Cash).xlsx
+++ b/Juan Alduey (Time Log and Petty Cash).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceciliametheny/repos/ceciliametheny/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{76FA4691-D726-BC46-AF3A-1CC6FA704EC5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CF477952-70D2-A348-9C0D-A6170322D373}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15840" xr2:uid="{33F21683-6D57-0047-AE38-A532DA1E1845}"/>
+    <workbookView xWindow="2840" yWindow="2520" windowWidth="27640" windowHeight="15840" xr2:uid="{33F21683-6D57-0047-AE38-A532DA1E1845}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeLog" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Refactoring code, submitting time log, determining git workflow</t>
   </si>
@@ -119,6 +119,15 @@
   </si>
   <si>
     <t>Fixed visa, date, and category buttons, plus data validation issue with LM transactions.</t>
+  </si>
+  <si>
+    <t>Collapsed LM transactions into one step.</t>
+  </si>
+  <si>
+    <t>Errorhandling for LM transactions</t>
+  </si>
+  <si>
+    <t>Errorhandling for LM transactions; Clarifying CM requests</t>
   </si>
 </sst>
 </file>
@@ -202,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -232,6 +241,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,6 +746,17 @@
             <v>2252</v>
           </cell>
         </row>
+        <row r="43">
+          <cell r="A43">
+            <v>41758</v>
+          </cell>
+          <cell r="B43" t="str">
+            <v>Grocery Store</v>
+          </cell>
+          <cell r="C43">
+            <v>80</v>
+          </cell>
+        </row>
         <row r="44">
           <cell r="A44">
             <v>41707</v>
@@ -954,6 +975,303 @@
           </cell>
           <cell r="C63">
             <v>2293.67</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64">
+            <v>41757</v>
+          </cell>
+          <cell r="B64" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C64">
+            <v>90</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65">
+            <v>41756</v>
+          </cell>
+          <cell r="B65" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C65">
+            <v>100</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66">
+            <v>41758</v>
+          </cell>
+          <cell r="B66" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C66">
+            <v>300</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67">
+            <v>41758</v>
+          </cell>
+          <cell r="B67" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C67">
+            <v>600</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68">
+            <v>41756</v>
+          </cell>
+          <cell r="B68" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C68">
+            <v>900</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69">
+            <v>41756</v>
+          </cell>
+          <cell r="B69" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C69">
+            <v>980</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70">
+            <v>41758</v>
+          </cell>
+          <cell r="B70" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C70">
+            <v>999</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71">
+            <v>41758</v>
+          </cell>
+          <cell r="B71" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C71">
+            <v>2454</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72">
+            <v>41758</v>
+          </cell>
+          <cell r="B72" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C72">
+            <v>333</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73">
+            <v>41757</v>
+          </cell>
+          <cell r="B73" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C73">
+            <v>1200</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74">
+            <v>41757</v>
+          </cell>
+          <cell r="B74" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C74">
+            <v>1200</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75">
+            <v>41757</v>
+          </cell>
+          <cell r="B75" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C75">
+            <v>1200</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76">
+            <v>41757</v>
+          </cell>
+          <cell r="B76" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C76">
+            <v>1200</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77">
+            <v>41757</v>
+          </cell>
+          <cell r="B77" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C77">
+            <v>1200</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78">
+            <v>41761</v>
+          </cell>
+          <cell r="B78" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C78">
+            <v>100</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79">
+            <v>41760</v>
+          </cell>
+          <cell r="B79" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C79">
+            <v>300</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80">
+            <v>41759</v>
+          </cell>
+          <cell r="B80" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C80">
+            <v>45</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81">
+            <v>41759</v>
+          </cell>
+          <cell r="B81" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C81">
+            <v>90</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82">
+            <v>41760</v>
+          </cell>
+          <cell r="B82" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C82">
+            <v>95</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83">
+            <v>41760</v>
+          </cell>
+          <cell r="B83" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C83">
+            <v>95</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84">
+            <v>41761</v>
+          </cell>
+          <cell r="B84" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C84">
+            <v>200</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85">
+            <v>41760</v>
+          </cell>
+          <cell r="B85" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C85">
+            <v>300</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86">
+            <v>41761</v>
+          </cell>
+          <cell r="B86" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C86">
+            <v>120</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="A87">
+            <v>41759</v>
+          </cell>
+          <cell r="B87" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C87">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="A88">
+            <v>41759</v>
+          </cell>
+          <cell r="B88" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C88">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="A89">
+            <v>41656</v>
+          </cell>
+          <cell r="B89" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C89">
+            <v>72.8</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="A90">
+            <v>41656</v>
+          </cell>
+          <cell r="B90" t="str">
+            <v>Lucille Metheny</v>
+          </cell>
+          <cell r="C90">
+            <v>72.8</v>
           </cell>
         </row>
       </sheetData>
@@ -5032,12 +5350,221 @@
         </row>
         <row r="372">
           <cell r="A372">
-            <v>41753</v>
+            <v>41739</v>
           </cell>
           <cell r="B372" t="str">
             <v>Food Out</v>
           </cell>
           <cell r="C372">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="373">
+          <cell r="A373">
+            <v>41757</v>
+          </cell>
+          <cell r="B373" t="str">
+            <v>Grocery Store</v>
+          </cell>
+          <cell r="C373">
+            <v>90</v>
+          </cell>
+        </row>
+        <row r="374">
+          <cell r="A374">
+            <v>41756</v>
+          </cell>
+          <cell r="B374" t="str">
+            <v>Business Travel</v>
+          </cell>
+          <cell r="C374">
+            <v>100</v>
+          </cell>
+        </row>
+        <row r="375">
+          <cell r="A375">
+            <v>41758</v>
+          </cell>
+          <cell r="B375" t="str">
+            <v>Grocery Store</v>
+          </cell>
+          <cell r="C375">
+            <v>300</v>
+          </cell>
+        </row>
+        <row r="376">
+          <cell r="A376">
+            <v>41758</v>
+          </cell>
+          <cell r="B376" t="str">
+            <v>Food Out</v>
+          </cell>
+          <cell r="C376">
+            <v>600</v>
+          </cell>
+        </row>
+        <row r="377">
+          <cell r="A377">
+            <v>41756</v>
+          </cell>
+          <cell r="B377" t="str">
+            <v>Office Supplies</v>
+          </cell>
+          <cell r="C377">
+            <v>900</v>
+          </cell>
+        </row>
+        <row r="378">
+          <cell r="A378">
+            <v>41756</v>
+          </cell>
+          <cell r="B378" t="str">
+            <v>Food Out</v>
+          </cell>
+          <cell r="C378">
+            <v>980</v>
+          </cell>
+        </row>
+        <row r="379">
+          <cell r="A379">
+            <v>41758</v>
+          </cell>
+          <cell r="B379" t="str">
+            <v>Grocery Store</v>
+          </cell>
+          <cell r="C379">
+            <v>999</v>
+          </cell>
+        </row>
+        <row r="380">
+          <cell r="A380">
+            <v>41758</v>
+          </cell>
+          <cell r="B380" t="str">
+            <v>Food Out</v>
+          </cell>
+          <cell r="C380">
+            <v>2454</v>
+          </cell>
+        </row>
+        <row r="381">
+          <cell r="A381">
+            <v>41758</v>
+          </cell>
+          <cell r="B381" t="str">
+            <v>Office Supplies</v>
+          </cell>
+          <cell r="C381">
+            <v>333</v>
+          </cell>
+        </row>
+        <row r="382">
+          <cell r="A382">
+            <v>41757</v>
+          </cell>
+          <cell r="B382" t="str">
+            <v>Food Out</v>
+          </cell>
+          <cell r="C382">
+            <v>1200</v>
+          </cell>
+        </row>
+        <row r="383">
+          <cell r="A383">
+            <v>41761</v>
+          </cell>
+          <cell r="B383" t="str">
+            <v>food Out</v>
+          </cell>
+          <cell r="C383">
+            <v>100</v>
+          </cell>
+        </row>
+        <row r="384">
+          <cell r="A384">
+            <v>41760</v>
+          </cell>
+          <cell r="B384" t="str">
+            <v>Grocery Store</v>
+          </cell>
+          <cell r="C384">
+            <v>300</v>
+          </cell>
+        </row>
+        <row r="385">
+          <cell r="A385">
+            <v>41759</v>
+          </cell>
+          <cell r="B385" t="str">
+            <v>Public Transit</v>
+          </cell>
+          <cell r="C385">
+            <v>45</v>
+          </cell>
+        </row>
+        <row r="386">
+          <cell r="A386">
+            <v>41759</v>
+          </cell>
+          <cell r="B386" t="str">
+            <v>Grocery Store</v>
+          </cell>
+          <cell r="C386">
+            <v>90</v>
+          </cell>
+        </row>
+        <row r="387">
+          <cell r="A387">
+            <v>41760</v>
+          </cell>
+          <cell r="B387" t="str">
+            <v>Food Out</v>
+          </cell>
+          <cell r="C387">
+            <v>95</v>
+          </cell>
+        </row>
+        <row r="388">
+          <cell r="A388">
+            <v>41761</v>
+          </cell>
+          <cell r="B388" t="str">
+            <v>Food Out</v>
+          </cell>
+          <cell r="C388">
+            <v>200</v>
+          </cell>
+        </row>
+        <row r="389">
+          <cell r="A389">
+            <v>41760</v>
+          </cell>
+          <cell r="B389" t="str">
+            <v>Food Out</v>
+          </cell>
+          <cell r="C389">
+            <v>300</v>
+          </cell>
+        </row>
+        <row r="390">
+          <cell r="A390">
+            <v>41761</v>
+          </cell>
+          <cell r="B390" t="str">
+            <v>Food Out</v>
+          </cell>
+          <cell r="C390">
+            <v>120</v>
+          </cell>
+        </row>
+        <row r="391">
+          <cell r="A391">
+            <v>41759</v>
+          </cell>
+          <cell r="B391" t="str">
+            <v>Public Transit</v>
+          </cell>
+          <cell r="C391">
             <v>35</v>
           </cell>
         </row>
@@ -5644,8 +6171,8 @@
   <sheetPr codeName="Sheet6" filterMode="1"/>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -5685,7 +6212,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ref="D2:D25" si="0">(C2-B2)*24</f>
+        <f t="shared" ref="D2:D28" si="0">(C2-B2)*24</f>
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -6106,19 +6633,59 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>43220</v>
       </c>
       <c r="B26" s="3">
         <v>0.44236111111111115</v>
       </c>
+      <c r="C26" s="3">
+        <v>0.62569444444444444</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>4.3999999999999986</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="16"/>
+    <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="19">
+        <v>43223</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.49583333333333335</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5666666666666664</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
+    <row r="28" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A28" s="17">
+        <v>43223</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.52638888888888891</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.60555555555555551</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8999999999999986</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="16"/>

</xml_diff>